<commit_message>
Cambios en la formula
</commit_message>
<xml_diff>
--- a/Transpo/Servicios.xlsx
+++ b/Transpo/Servicios.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\douglas.vega\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Transpo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA0647C-193E-49E5-AF27-2CA3F1EC06B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>Paquete 1</t>
   </si>
@@ -108,14 +107,29 @@
   </si>
   <si>
     <t>Cobro Total</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Polizas Aparte</t>
+  </si>
+  <si>
+    <t>Con factura</t>
+  </si>
+  <si>
+    <t>Si nosotros importamos = 4%</t>
+  </si>
+  <si>
+    <t>Si ellos importan = 15%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-540A]* #,##0.00_ ;_-[$$-540A]* \-#,##0.00\ ;_-[$$-540A]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -290,12 +304,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -310,15 +324,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Énfasis5" xfId="1" builtinId="48"/>
@@ -600,11 +615,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H8" sqref="H8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,17 +633,17 @@
     <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -659,7 +674,7 @@
       <c r="V6" s="8"/>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="F7" s="6"/>
       <c r="M7" s="6"/>
@@ -668,12 +683,12 @@
       </c>
       <c r="W7" s="11"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>50000</v>
+        <v>2000</v>
       </c>
       <c r="F8" s="6"/>
       <c r="H8" t="s">
@@ -687,14 +702,23 @@
         <v>2</v>
       </c>
       <c r="S8" s="1">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="U8" t="s">
         <v>17</v>
       </c>
       <c r="W8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8">
+        <v>15</v>
+      </c>
+      <c r="Z8" s="28">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
@@ -703,18 +727,18 @@
       </c>
       <c r="E9" s="1">
         <f>E8*C9</f>
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="F9" s="6"/>
       <c r="H9" t="s">
         <v>3</v>
       </c>
       <c r="J9" s="2">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="L9" s="1">
         <f>L8*J9</f>
-        <v>208</v>
+        <v>240</v>
       </c>
       <c r="M9" s="6"/>
       <c r="O9" t="s">
@@ -725,14 +749,14 @@
       </c>
       <c r="S9" s="1">
         <f>IF(S8&lt;=10000,S8*Q9,IF(S8&lt;=20000,S8*(((Q9*100)-0.5)/100),IF(S8&lt;=50000,S8*(((Q9*100)-1)/100),IF(S8&lt;=100000,S8*(((Q9*100)-1.5)/100),S8*(((Q9*100)-2)/100)))))</f>
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="U9" t="s">
         <v>18</v>
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
@@ -741,7 +765,7 @@
       <c r="D10" s="26"/>
       <c r="E10" s="27">
         <f>E8+E9</f>
-        <v>55000</v>
+        <v>2200</v>
       </c>
       <c r="F10" s="6"/>
       <c r="H10" s="26" t="s">
@@ -752,7 +776,7 @@
       <c r="K10" s="26"/>
       <c r="L10" s="27">
         <f>L8+L9</f>
-        <v>1808</v>
+        <v>1840</v>
       </c>
       <c r="M10" s="6"/>
       <c r="O10" s="26" t="s">
@@ -763,14 +787,20 @@
       <c r="R10" s="26"/>
       <c r="S10" s="27">
         <f>S9</f>
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="U10" t="s">
         <v>19</v>
       </c>
       <c r="W10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>4</v>
       </c>
@@ -783,7 +813,7 @@
       </c>
       <c r="L11" s="1">
         <f>L10*J11</f>
-        <v>90.4</v>
+        <v>92</v>
       </c>
       <c r="M11" s="6"/>
       <c r="O11" t="s">
@@ -794,7 +824,7 @@
       </c>
       <c r="W11" s="6"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="F12" s="6"/>
       <c r="M12" s="6"/>
@@ -802,8 +832,14 @@
         <v>21</v>
       </c>
       <c r="W12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z12" s="28">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>5</v>
       </c>
@@ -812,7 +848,7 @@
       <c r="D13" s="24"/>
       <c r="E13" s="25">
         <f>E9</f>
-        <v>5000</v>
+        <v>200</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="12"/>
@@ -824,7 +860,7 @@
       <c r="K13" s="24"/>
       <c r="L13" s="25">
         <f>L9-L11</f>
-        <v>117.6</v>
+        <v>148</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="12"/>
@@ -836,14 +872,14 @@
       <c r="R13" s="24"/>
       <c r="S13" s="25">
         <f>S9</f>
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -851,7 +887,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>24</v>
       </c>
@@ -860,11 +896,11 @@
       <c r="D15" s="18"/>
       <c r="E15" s="19">
         <f>E10+L10+S10</f>
-        <v>58308</v>
+        <v>4440</v>
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
@@ -873,8 +909,11 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>10</v>
       </c>
@@ -883,24 +922,30 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22">
         <f>E13+L13+S13</f>
-        <v>6617.6</v>
+        <v>748</v>
       </c>
       <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="10"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>1</v>
       </c>
@@ -922,7 +967,7 @@
       <c r="O23" s="8"/>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -942,7 +987,7 @@
       <c r="O24" s="3"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>2</v>
       </c>
@@ -961,7 +1006,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="4">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3" t="s">
@@ -970,7 +1015,7 @@
       <c r="O25" s="3"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>3</v>
       </c>
@@ -995,7 +1040,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="4">
         <f>IF(L25&lt;=10000,L25*J26,IF(L25&lt;=20000,L25*(((J26*100)-0.5)/100),IF(L25&lt;=50000,L25*(((J26*100)-1)/100),IF(L25&lt;=100000,L25*(((J26*100)-1.5)/100),L25*(((J26*100)-2)/100)))))</f>
-        <v>700.00000000000011</v>
+        <v>400</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3" t="s">
@@ -1004,7 +1049,7 @@
       <c r="O26" s="3"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>14</v>
       </c>
@@ -1025,7 +1070,7 @@
       <c r="K27" s="18"/>
       <c r="L27" s="19">
         <f>L26</f>
-        <v>700.00000000000011</v>
+        <v>400</v>
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3" t="s">
@@ -1034,7 +1079,7 @@
       <c r="O27" s="3"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +1108,7 @@
       <c r="O28" s="3"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1083,7 +1128,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>5</v>
       </c>
@@ -1104,14 +1149,14 @@
       <c r="K30" s="24"/>
       <c r="L30" s="25">
         <f>L26</f>
-        <v>700.00000000000011</v>
+        <v>400</v>
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1129,7 +1174,7 @@
       <c r="O31" s="16"/>
       <c r="P31" s="16"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>24</v>
       </c>
@@ -1138,7 +1183,7 @@
       <c r="D32" s="18"/>
       <c r="E32" s="19">
         <f>E27+L27</f>
-        <v>2508</v>
+        <v>2208</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="13"/>
@@ -1181,7 +1226,7 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22">
         <f>E30+L30</f>
-        <v>817.60000000000014</v>
+        <v>517.6</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="13"/>

</xml_diff>